<commit_message>
End of summer update
</commit_message>
<xml_diff>
--- a/uv_fluxes.xlsx
+++ b/uv_fluxes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiemel/Desktop/NASA_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173F670D-4E64-7A4C-99DD-6456939441F0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7566CE48-5BBE-E84B-9E78-F1450A8A6052}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{942B6D15-DAF8-BF42-97C8-ECF2BB5E6A39}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15000" xr2:uid="{942B6D15-DAF8-BF42-97C8-ECF2BB5E6A39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="156">
   <si>
     <t>SiIII_flux</t>
   </si>
@@ -499,7 +499,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -559,6 +559,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF9900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -580,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -594,6 +613,9 @@
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,8 +932,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0202CB-48C7-494E-B0A3-04A5E53E516A}">
   <dimension ref="A1:X112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X98" sqref="X98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1638,17 +1661,17 @@
       <c r="L13" t="s">
         <v>46</v>
       </c>
-      <c r="M13" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" t="s">
-        <v>46</v>
-      </c>
-      <c r="O13" t="s">
-        <v>46</v>
-      </c>
-      <c r="P13" t="s">
-        <v>46</v>
+      <c r="M13" s="15">
+        <v>4.1800000000000001E-15</v>
+      </c>
+      <c r="N13" s="15">
+        <v>1.4799999999999999E-16</v>
+      </c>
+      <c r="O13" s="8">
+        <v>1.2199999999999999E-14</v>
+      </c>
+      <c r="P13" s="8">
+        <v>2.9999999999999999E-16</v>
       </c>
       <c r="Q13" t="s">
         <v>46</v>
@@ -1710,17 +1733,17 @@
       <c r="L14" t="s">
         <v>46</v>
       </c>
-      <c r="M14" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" t="s">
-        <v>46</v>
-      </c>
-      <c r="P14" t="s">
-        <v>46</v>
+      <c r="M14" s="15">
+        <v>8.3E-14</v>
+      </c>
+      <c r="N14" s="15">
+        <v>1.15E-15</v>
+      </c>
+      <c r="O14" s="7">
+        <v>9.1399999999999994E-14</v>
+      </c>
+      <c r="P14" s="7">
+        <v>1.0000000000000001E-15</v>
       </c>
       <c r="Q14" t="s">
         <v>46</v>
@@ -1782,17 +1805,17 @@
       <c r="L15" t="s">
         <v>46</v>
       </c>
-      <c r="M15" t="s">
-        <v>46</v>
-      </c>
-      <c r="N15" t="s">
-        <v>46</v>
-      </c>
-      <c r="O15" t="s">
-        <v>46</v>
-      </c>
-      <c r="P15" t="s">
-        <v>46</v>
+      <c r="M15" s="15">
+        <v>1.2300000000000001E-15</v>
+      </c>
+      <c r="N15" s="15">
+        <v>9.6899999999999994E-17</v>
+      </c>
+      <c r="O15" s="7">
+        <v>4.4999999999999998E-15</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2E-16</v>
       </c>
       <c r="Q15" t="s">
         <v>46</v>
@@ -1854,17 +1877,17 @@
       <c r="L16" t="s">
         <v>46</v>
       </c>
-      <c r="M16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O16" t="s">
-        <v>46</v>
-      </c>
-      <c r="P16" t="s">
-        <v>46</v>
+      <c r="M16" s="15">
+        <v>5.58E-15</v>
+      </c>
+      <c r="N16" s="15">
+        <v>2.1199999999999999E-16</v>
+      </c>
+      <c r="O16" s="7">
+        <v>1.1799999999999999E-14</v>
+      </c>
+      <c r="P16" s="1">
+        <v>2.9999999999999999E-16</v>
       </c>
       <c r="Q16" t="s">
         <v>46</v>
@@ -2106,11 +2129,11 @@
       <c r="X19" s="4"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+      <c r="A20" s="15">
+        <v>5.1700000000000002E-16</v>
+      </c>
+      <c r="B20" s="15">
+        <v>4.2299999999999998E-17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>46</v>
@@ -2124,11 +2147,11 @@
       <c r="F20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>46</v>
+      <c r="G20" s="15">
+        <v>8.5499999999999999E-16</v>
+      </c>
+      <c r="H20" s="15">
+        <v>8.1700000000000001E-17</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>46</v>
@@ -2136,29 +2159,29 @@
       <c r="J20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>46</v>
+      <c r="K20" s="15">
+        <v>5.1800000000000004E-16</v>
+      </c>
+      <c r="L20" s="15">
+        <v>6.1800000000000001E-17</v>
+      </c>
+      <c r="M20" s="15">
+        <v>2.0200000000000001E-15</v>
+      </c>
+      <c r="N20" s="15">
+        <v>2.4499999999999999E-16</v>
+      </c>
+      <c r="O20" s="15">
+        <v>2.7300000000000002E-15</v>
+      </c>
+      <c r="P20" s="15">
+        <v>2.1799999999999999E-16</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>5.1499999999999999E-16</v>
+      </c>
+      <c r="R20" s="15">
+        <v>3.8600000000000001E-17</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>46</v>
@@ -2682,11 +2705,11 @@
       <c r="X27" s="4"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>46</v>
+      <c r="A28" s="15">
+        <v>3.3200000000000002E-16</v>
+      </c>
+      <c r="B28" s="15">
+        <v>3.39E-17</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -2700,11 +2723,11 @@
       <c r="F28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>46</v>
+      <c r="G28" s="15">
+        <v>7.0699999999999995E-16</v>
+      </c>
+      <c r="H28" s="15">
+        <v>7.2499999999999995E-17</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>46</v>
@@ -2712,29 +2735,29 @@
       <c r="J28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R28" s="4" t="s">
-        <v>46</v>
+      <c r="K28" s="15">
+        <v>3.9299999999999998E-16</v>
+      </c>
+      <c r="L28" s="15">
+        <v>6.3899999999999998E-14</v>
+      </c>
+      <c r="M28" s="15">
+        <v>1.75E-15</v>
+      </c>
+      <c r="N28" s="15">
+        <v>9.1E-17</v>
+      </c>
+      <c r="O28" s="15">
+        <v>2.1400000000000001E-15</v>
+      </c>
+      <c r="P28" s="15">
+        <v>7.8200000000000006E-17</v>
+      </c>
+      <c r="Q28" s="15">
+        <v>6.8999999999999997E-16</v>
+      </c>
+      <c r="R28" s="15">
+        <v>4.4E-17</v>
       </c>
       <c r="S28" t="s">
         <v>46</v>
@@ -2898,11 +2921,11 @@
       <c r="X30" s="4"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>46</v>
+      <c r="A31" s="15">
+        <v>1.41E-15</v>
+      </c>
+      <c r="B31" s="15">
+        <v>4.6600000000000002E-17</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
@@ -2916,41 +2939,41 @@
       <c r="F31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R31" s="3" t="s">
-        <v>46</v>
+      <c r="G31" s="15">
+        <v>2.9499999999999998E-15</v>
+      </c>
+      <c r="H31" s="15">
+        <v>9.1E-17</v>
+      </c>
+      <c r="I31" s="15">
+        <v>5.1799999999999998E-14</v>
+      </c>
+      <c r="J31" s="15">
+        <v>4.25E-15</v>
+      </c>
+      <c r="K31" s="15">
+        <v>1.2900000000000001E-15</v>
+      </c>
+      <c r="L31" s="15">
+        <v>6.3100000000000005E-17</v>
+      </c>
+      <c r="M31" s="15">
+        <v>3.47E-15</v>
+      </c>
+      <c r="N31" s="15">
+        <v>1.07E-16</v>
+      </c>
+      <c r="O31" s="15">
+        <v>5.6000000000000003E-15</v>
+      </c>
+      <c r="P31" s="15">
+        <v>1.4300000000000001E-16</v>
+      </c>
+      <c r="Q31" s="15">
+        <v>1.8599999999999999E-15</v>
+      </c>
+      <c r="R31" s="15">
+        <v>4.2700000000000002E-17</v>
       </c>
       <c r="S31" t="s">
         <v>46</v>
@@ -2970,11 +2993,11 @@
       <c r="X31" s="4"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>46</v>
+      <c r="A32" s="15">
+        <v>6.36E-15</v>
+      </c>
+      <c r="B32" s="15">
+        <v>1.97E-16</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>46</v>
@@ -2988,11 +3011,11 @@
       <c r="F32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>46</v>
+      <c r="G32" s="15">
+        <v>9.5600000000000007E-15</v>
+      </c>
+      <c r="H32" s="15">
+        <v>3.6800000000000001E-16</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>46</v>
@@ -3000,29 +3023,29 @@
       <c r="J32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R32" s="3" t="s">
-        <v>46</v>
+      <c r="K32" s="15">
+        <v>7.5699999999999996E-15</v>
+      </c>
+      <c r="L32" s="15">
+        <v>3.1000000000000001E-16</v>
+      </c>
+      <c r="M32" s="15">
+        <v>2.19E-14</v>
+      </c>
+      <c r="N32" s="15">
+        <v>8.0800000000000001E-16</v>
+      </c>
+      <c r="O32" s="15">
+        <v>3.6400000000000001E-14</v>
+      </c>
+      <c r="P32" s="15">
+        <v>1.02E-15</v>
+      </c>
+      <c r="Q32" s="15">
+        <v>5.0399999999999999E-15</v>
+      </c>
+      <c r="R32" s="15">
+        <v>1.47E-16</v>
       </c>
       <c r="S32" t="s">
         <v>46</v>
@@ -5130,11 +5153,11 @@
       <c r="X61" s="4"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62" t="s">
-        <v>46</v>
+      <c r="A62" s="15">
+        <v>3.2699999999999999E-16</v>
+      </c>
+      <c r="B62" s="15">
+        <v>1.0600000000000001E-17</v>
       </c>
       <c r="C62" t="s">
         <v>46</v>
@@ -5148,11 +5171,11 @@
       <c r="F62" t="s">
         <v>46</v>
       </c>
-      <c r="G62" t="s">
-        <v>46</v>
-      </c>
-      <c r="H62" t="s">
-        <v>46</v>
+      <c r="G62" s="15">
+        <v>6.4600000000000004E-16</v>
+      </c>
+      <c r="H62" s="15">
+        <v>2.14E-17</v>
       </c>
       <c r="I62" t="s">
         <v>46</v>
@@ -5160,11 +5183,11 @@
       <c r="J62" t="s">
         <v>46</v>
       </c>
-      <c r="K62" t="s">
-        <v>46</v>
-      </c>
-      <c r="L62" t="s">
-        <v>46</v>
+      <c r="K62" s="15">
+        <v>3.58E-16</v>
+      </c>
+      <c r="L62" s="15">
+        <v>1.65E-17</v>
       </c>
       <c r="M62" t="s">
         <v>46</v>
@@ -5178,11 +5201,11 @@
       <c r="P62" t="s">
         <v>46</v>
       </c>
-      <c r="Q62" t="s">
-        <v>46</v>
-      </c>
-      <c r="R62" t="s">
-        <v>46</v>
+      <c r="Q62" s="15">
+        <v>6.5999999999999998E-16</v>
+      </c>
+      <c r="R62" s="15">
+        <v>1.31E-17</v>
       </c>
       <c r="S62" t="s">
         <v>46</v>
@@ -5343,11 +5366,11 @@
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>46</v>
-      </c>
-      <c r="B65" t="s">
-        <v>46</v>
+      <c r="A65" s="8">
+        <v>7.0000000000000001E-15</v>
+      </c>
+      <c r="B65" s="8">
+        <v>1.6E-15</v>
       </c>
       <c r="C65" t="s">
         <v>46</v>
@@ -5361,11 +5384,11 @@
       <c r="F65" t="s">
         <v>46</v>
       </c>
-      <c r="G65" t="s">
-        <v>46</v>
-      </c>
-      <c r="H65" t="s">
-        <v>46</v>
+      <c r="G65" s="8">
+        <v>1.66E-14</v>
+      </c>
+      <c r="H65" s="8">
+        <v>2.5E-15</v>
       </c>
       <c r="I65" t="s">
         <v>46</v>
@@ -5373,11 +5396,11 @@
       <c r="J65" t="s">
         <v>46</v>
       </c>
-      <c r="K65" t="s">
-        <v>46</v>
-      </c>
-      <c r="L65" t="s">
-        <v>46</v>
+      <c r="K65" s="8">
+        <v>2.6399999999999999E-15</v>
+      </c>
+      <c r="L65" s="8">
+        <v>7.3999999999999999E-16</v>
       </c>
       <c r="M65" t="s">
         <v>46</v>
@@ -5415,11 +5438,11 @@
       <c r="X65" s="4"/>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>46</v>
-      </c>
-      <c r="B66" t="s">
-        <v>46</v>
+      <c r="A66" s="8">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="B66" s="8">
+        <v>1.3E-15</v>
       </c>
       <c r="C66" t="s">
         <v>46</v>
@@ -5433,11 +5456,11 @@
       <c r="F66" t="s">
         <v>46</v>
       </c>
-      <c r="G66" t="s">
-        <v>46</v>
-      </c>
-      <c r="H66" t="s">
-        <v>46</v>
+      <c r="G66" s="8">
+        <v>1.58E-14</v>
+      </c>
+      <c r="H66" s="8">
+        <v>2.1999999999999999E-15</v>
       </c>
       <c r="I66" t="s">
         <v>46</v>
@@ -5445,11 +5468,11 @@
       <c r="J66" t="s">
         <v>46</v>
       </c>
-      <c r="K66" t="s">
-        <v>46</v>
-      </c>
-      <c r="L66" t="s">
-        <v>46</v>
+      <c r="K66" s="8">
+        <v>2.67E-15</v>
+      </c>
+      <c r="L66" s="8">
+        <v>6.7000000000000004E-16</v>
       </c>
       <c r="M66" t="s">
         <v>46</v>
@@ -5487,11 +5510,11 @@
       <c r="X66" s="4"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B67" t="s">
-        <v>46</v>
+      <c r="A67" s="8">
+        <v>1.42E-14</v>
+      </c>
+      <c r="B67" s="8">
+        <v>2.6E-15</v>
       </c>
       <c r="C67" t="s">
         <v>46</v>
@@ -5505,11 +5528,11 @@
       <c r="F67" t="s">
         <v>46</v>
       </c>
-      <c r="G67" t="s">
-        <v>46</v>
-      </c>
-      <c r="H67" t="s">
-        <v>46</v>
+      <c r="G67" s="8">
+        <v>3.02E-14</v>
+      </c>
+      <c r="H67" s="8">
+        <v>3.8000000000000002E-15</v>
       </c>
       <c r="I67" t="s">
         <v>46</v>
@@ -5517,11 +5540,11 @@
       <c r="J67" t="s">
         <v>46</v>
       </c>
-      <c r="K67" t="s">
-        <v>46</v>
-      </c>
-      <c r="L67" t="s">
-        <v>46</v>
+      <c r="K67" s="8">
+        <v>5.6000000000000003E-15</v>
+      </c>
+      <c r="L67" s="8">
+        <v>1.2E-15</v>
       </c>
       <c r="M67" t="s">
         <v>46</v>
@@ -5550,10 +5573,10 @@
       <c r="U67" s="4">
         <v>0.59</v>
       </c>
-      <c r="V67" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="W67" t="s">
+      <c r="V67" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="W67" s="14" t="s">
         <v>110</v>
       </c>
       <c r="X67" s="4"/>
@@ -5577,11 +5600,11 @@
       <c r="F68" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G68" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>46</v>
+      <c r="G68" s="7">
+        <v>2.7000000000000001E-17</v>
+      </c>
+      <c r="H68" s="7">
+        <v>2.2E-17</v>
       </c>
       <c r="I68" s="4" t="s">
         <v>46</v>
@@ -5589,11 +5612,11 @@
       <c r="J68" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K68" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L68" s="4" t="s">
-        <v>46</v>
+      <c r="K68" s="7">
+        <v>1.3E-17</v>
+      </c>
+      <c r="L68" s="7">
+        <v>1.5E-17</v>
       </c>
       <c r="M68" s="4" t="s">
         <v>46</v>
@@ -5601,11 +5624,11 @@
       <c r="N68" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O68" s="4" t="s">
-        <v>46</v>
+      <c r="O68" s="7">
+        <v>7.1E-16</v>
       </c>
       <c r="P68" s="7">
-        <v>7.1E-16</v>
+        <v>6.0000000000000001E-17</v>
       </c>
       <c r="Q68" s="4" t="s">
         <v>46</v>
@@ -5622,10 +5645,10 @@
       <c r="U68" s="4">
         <v>0.11</v>
       </c>
-      <c r="V68" t="s">
-        <v>46</v>
-      </c>
-      <c r="W68" t="s">
+      <c r="V68" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="W68" s="14" t="s">
         <v>111</v>
       </c>
       <c r="X68" s="4"/>
@@ -5649,11 +5672,11 @@
       <c r="F69" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G69" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H69" s="4" t="s">
-        <v>46</v>
+      <c r="G69" s="7">
+        <v>6.9E-17</v>
+      </c>
+      <c r="H69" s="7">
+        <v>4.0000000000000003E-17</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>46</v>
@@ -5661,11 +5684,11 @@
       <c r="J69" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K69" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L69" s="4" t="s">
-        <v>46</v>
+      <c r="K69" s="7">
+        <v>1.6000000000000001E-17</v>
+      </c>
+      <c r="L69" s="7">
+        <v>2.3000000000000001E-17</v>
       </c>
       <c r="M69" s="4" t="s">
         <v>46</v>
@@ -5676,7 +5699,9 @@
       <c r="O69" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P69" s="4"/>
+      <c r="P69" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="Q69" s="4" t="s">
         <v>46</v>
       </c>
@@ -5692,38 +5717,38 @@
       <c r="U69" s="4">
         <v>0.12</v>
       </c>
-      <c r="V69" t="s">
-        <v>46</v>
-      </c>
-      <c r="W69" t="s">
+      <c r="V69" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="W69" s="14" t="s">
         <v>112</v>
       </c>
       <c r="X69" s="4"/>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
-        <v>0</v>
-      </c>
-      <c r="B70" s="3">
-        <v>0</v>
-      </c>
-      <c r="C70" s="3">
-        <v>0</v>
-      </c>
-      <c r="D70" s="3">
-        <v>0</v>
-      </c>
-      <c r="E70" s="3">
-        <v>0</v>
-      </c>
-      <c r="F70" s="3">
-        <v>0</v>
-      </c>
-      <c r="G70" s="3">
-        <v>0</v>
-      </c>
-      <c r="H70" s="3">
-        <v>0</v>
+      <c r="A70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="I70" s="1">
         <v>1.1E-12</v>
@@ -5731,32 +5756,32 @@
       <c r="J70" s="1">
         <v>1.42E-15</v>
       </c>
-      <c r="K70" s="3">
-        <v>0</v>
-      </c>
-      <c r="L70" s="3">
-        <v>0</v>
-      </c>
-      <c r="M70" s="3">
-        <v>0</v>
-      </c>
-      <c r="N70" s="3">
-        <v>0</v>
-      </c>
-      <c r="O70" s="3">
-        <v>0</v>
-      </c>
-      <c r="P70" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q70" s="3">
-        <v>0</v>
-      </c>
-      <c r="R70" s="3">
-        <v>0</v>
-      </c>
-      <c r="S70" s="3">
-        <v>0</v>
+      <c r="K70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="T70" s="3">
         <v>5.99</v>
@@ -5815,11 +5840,11 @@
       <c r="N71" t="s">
         <v>46</v>
       </c>
-      <c r="O71" t="s">
-        <v>46</v>
+      <c r="O71" s="8">
+        <v>2.8000000000000001E-15</v>
       </c>
       <c r="P71" s="7">
-        <v>2.8000000000000001E-15</v>
+        <v>9.9999999999999998E-17</v>
       </c>
       <c r="Q71" t="s">
         <v>46</v>
@@ -5887,11 +5912,11 @@
       <c r="N72" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O72" s="4" t="s">
-        <v>46</v>
+      <c r="O72" s="7">
+        <v>1.4000000000000001E-15</v>
       </c>
       <c r="P72" s="7">
-        <v>1.4000000000000001E-15</v>
+        <v>9.9999999999999998E-17</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>46</v>
@@ -5959,11 +5984,11 @@
       <c r="N73" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O73" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P73" s="4" t="s">
-        <v>46</v>
+      <c r="O73" s="15">
+        <v>4.7199999999999998E-16</v>
+      </c>
+      <c r="P73" s="15">
+        <v>4.4099999999999998E-17</v>
       </c>
       <c r="Q73" s="4" t="s">
         <v>46</v>
@@ -6058,11 +6083,11 @@
       <c r="X74" s="4"/>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>46</v>
+      <c r="A75" s="15">
+        <v>6.7400000000000001E-16</v>
+      </c>
+      <c r="B75" s="15">
+        <v>2.8299999999999999E-17</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>46</v>
@@ -6070,17 +6095,17 @@
       <c r="D75" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E75" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>46</v>
+      <c r="E75" s="15">
+        <v>8.9100000000000008E-16</v>
+      </c>
+      <c r="F75" s="15">
+        <v>6.5599999999999996E-17</v>
+      </c>
+      <c r="G75" s="15">
+        <v>7.4800000000000001E-15</v>
+      </c>
+      <c r="H75" s="15">
+        <v>1.38E-16</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>46</v>
@@ -6106,11 +6131,11 @@
       <c r="P75" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q75" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R75" s="4" t="s">
-        <v>46</v>
+      <c r="Q75" s="15">
+        <v>5.4799999999999999E-15</v>
+      </c>
+      <c r="R75" s="15">
+        <v>7.1500000000000003E-17</v>
       </c>
       <c r="S75" s="4" t="s">
         <v>46</v>
@@ -6202,11 +6227,11 @@
       <c r="X76" s="4"/>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>46</v>
+      <c r="A77" s="15">
+        <v>1.08E-15</v>
+      </c>
+      <c r="B77" s="15">
+        <v>3.0200000000000003E-17</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>46</v>
@@ -6214,17 +6239,17 @@
       <c r="D77" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>46</v>
+      <c r="E77" s="15">
+        <v>6.8399999999999997E-16</v>
+      </c>
+      <c r="F77" s="15">
+        <v>4.31E-17</v>
+      </c>
+      <c r="G77" s="15">
+        <v>4.3999999999999997E-15</v>
+      </c>
+      <c r="H77" s="15">
+        <v>7.2799999999999995E-17</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>46</v>
@@ -6250,11 +6275,11 @@
       <c r="P77" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q77" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R77" s="4" t="s">
-        <v>46</v>
+      <c r="Q77" s="15">
+        <v>2.5899999999999999E-15</v>
+      </c>
+      <c r="R77" s="15">
+        <v>3.4700000000000002E-17</v>
       </c>
       <c r="S77" s="4" t="s">
         <v>46</v>
@@ -6418,11 +6443,11 @@
       <c r="X79" s="4"/>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>46</v>
+      <c r="A80" s="15">
+        <v>2.7700000000000001E-14</v>
+      </c>
+      <c r="B80" s="15">
+        <v>4.4600000000000005E-16</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>46</v>
@@ -6430,17 +6455,17 @@
       <c r="D80" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E80" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>46</v>
+      <c r="E80" s="15">
+        <v>3.6899999999999996E-15</v>
+      </c>
+      <c r="F80" s="15">
+        <v>1.56E-16</v>
+      </c>
+      <c r="G80" s="15">
+        <v>2.6999999999999999E-14</v>
+      </c>
+      <c r="H80" s="15">
+        <v>4.9800000000000001E-16</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>46</v>
@@ -6466,11 +6491,11 @@
       <c r="P80" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q80" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R80" s="4" t="s">
-        <v>46</v>
+      <c r="Q80" s="15">
+        <v>2.1399999999999999E-14</v>
+      </c>
+      <c r="R80" s="15">
+        <v>2.02E-16</v>
       </c>
       <c r="S80" s="4" t="s">
         <v>46</v>
@@ -6778,11 +6803,11 @@
       <c r="X84" s="4"/>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>46</v>
+      <c r="A85" s="15">
+        <v>1.5699999999999999E-14</v>
+      </c>
+      <c r="B85" s="15">
+        <v>8.8499999999999998E-16</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>46</v>

</xml_diff>